<commit_message>
Charts improved, Settings improved, Saving and Loading integrated, Input-Data added
</commit_message>
<xml_diff>
--- a/Dokumentation/Noctua_Zeitaufzeichnung.xlsx
+++ b/Dokumentation/Noctua_Zeitaufzeichnung.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="48" yWindow="0" windowWidth="20736" windowHeight="11760" activeTab="3"/>
+    <workbookView xWindow="48" yWindow="0" windowWidth="20736" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Gesamtstatus" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="126">
   <si>
     <t>Arbeitspaket</t>
   </si>
@@ -378,6 +378,30 @@
   </si>
   <si>
     <t>Testprogramm fertiggestellt</t>
+  </si>
+  <si>
+    <t>Graphische Darstellung der Charts um Candlesticks erweitert</t>
+  </si>
+  <si>
+    <t>Candlestick-Charts</t>
+  </si>
+  <si>
+    <t>Indikatoren in die die Chartsdarstellung integriert</t>
+  </si>
+  <si>
+    <t>Viusualisierung der Indikatoren</t>
+  </si>
+  <si>
+    <t>Speichern &amp; Laden möglich</t>
+  </si>
+  <si>
+    <t>Speichern und Laden ermöglichen</t>
+  </si>
+  <si>
+    <t>Order-Settings-Screen design</t>
+  </si>
+  <si>
+    <t>Order-Settings-Screen 20%</t>
   </si>
 </sst>
 </file>
@@ -954,12 +978,12 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:shape val="box"/>
-        <c:axId val="38553472"/>
-        <c:axId val="38555008"/>
+        <c:axId val="53106560"/>
+        <c:axId val="53108096"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="38553472"/>
+        <c:axId val="53106560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -968,7 +992,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38555008"/>
+        <c:crossAx val="53108096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -976,7 +1000,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="38555008"/>
+        <c:axId val="53108096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -992,7 +1016,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="38553472"/>
+        <c:crossAx val="53106560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1114,7 +1138,7 @@
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43</c:v>
+                  <c:v>61.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>48.5</c:v>
@@ -1133,12 +1157,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="38588416"/>
-        <c:axId val="38589952"/>
+        <c:axId val="53141504"/>
+        <c:axId val="53143040"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="38588416"/>
+        <c:axId val="53141504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1147,7 +1171,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38589952"/>
+        <c:crossAx val="53143040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1155,7 +1179,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="38589952"/>
+        <c:axId val="53143040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1166,7 +1190,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38588416"/>
+        <c:crossAx val="53141504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1580,7 +1604,7 @@
       </c>
       <c r="B3" s="7">
         <f>SUM(B6,B12,B27)</f>
-        <v>72</v>
+        <v>90.5</v>
       </c>
       <c r="C3" s="27">
         <f>AVERAGE(C6,C12,C17,C22,C27)</f>
@@ -1718,7 +1742,7 @@
       </c>
       <c r="B12" s="17">
         <f>BacktestingSoftware!J6</f>
-        <v>69</v>
+        <v>87.5</v>
       </c>
       <c r="C12" s="29">
         <f>SUM(C13:C16)</f>
@@ -1737,7 +1761,7 @@
       </c>
       <c r="B13" s="19">
         <f>BacktestingSoftware!J2</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C13" s="31">
         <v>0</v>
@@ -1753,7 +1777,7 @@
       </c>
       <c r="B14" s="19">
         <f>BacktestingSoftware!J3</f>
-        <v>14.5</v>
+        <v>29</v>
       </c>
       <c r="C14" s="31">
         <v>0</v>
@@ -2021,7 +2045,7 @@
       <c r="C35" s="42"/>
       <c r="D35" s="9">
         <f>SUM(Projektmanagment!I14,BacktestingSoftware!I14,Algorithmus!I14,Marktzustandserkennung!I14,Testing_Abschluss!I14)</f>
-        <v>43</v>
+        <v>61.5</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2328,10 +2352,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2397,7 +2421,7 @@
       <c r="I2" s="61"/>
       <c r="J2" s="35">
         <f>SUMIF(B:B,H2,E:E)</f>
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -2425,7 +2449,7 @@
       <c r="I3" s="61"/>
       <c r="J3" s="35">
         <f>SUMIF(B:B,H3,E:E)</f>
-        <v>14.5</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -2509,7 +2533,7 @@
       <c r="I6" s="58"/>
       <c r="J6" s="7">
         <f>SUM(J2:J5)</f>
-        <v>69</v>
+        <v>87.5</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -2686,10 +2710,10 @@
       </c>
       <c r="I14" s="35">
         <f>SUMIF(A:A,H14,E:E)</f>
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>61.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
@@ -2796,6 +2820,86 @@
       </c>
       <c r="F19" s="3" t="s">
         <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D20" s="1">
+        <v>41284</v>
+      </c>
+      <c r="E20" s="26">
+        <v>8</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21" s="1">
+        <v>41285</v>
+      </c>
+      <c r="E21" s="26">
+        <v>2</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D22" s="1">
+        <v>41286</v>
+      </c>
+      <c r="E22" s="26">
+        <v>4</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D23" s="1">
+        <v>41290</v>
+      </c>
+      <c r="E23" s="26">
+        <v>4.5</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2829,8 +2933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Finished Order-Settings-Design, Added Trendstregth Weighting and Updated ZeitNoctua_Zeitaufzeichnung
</commit_message>
<xml_diff>
--- a/Dokumentation/Noctua_Zeitaufzeichnung.xlsx
+++ b/Dokumentation/Noctua_Zeitaufzeichnung.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="130">
   <si>
     <t>Arbeitspaket</t>
   </si>
@@ -401,7 +401,19 @@
     <t>Order-Settings-Screen design</t>
   </si>
   <si>
-    <t>Order-Settings-Screen 20%</t>
+    <t>Verschiedene Trendstärken in die Performancemessung integriert</t>
+  </si>
+  <si>
+    <t>Trendstärken-Berechnungsmodell erstellt</t>
+  </si>
+  <si>
+    <t>Berechnungsmodell erstellt</t>
+  </si>
+  <si>
+    <t>Trendstärken integriert 80%</t>
+  </si>
+  <si>
+    <t>Order-Settings-Screen 40%</t>
   </si>
 </sst>
 </file>
@@ -978,12 +990,12 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:shape val="box"/>
-        <c:axId val="53106560"/>
-        <c:axId val="53108096"/>
+        <c:axId val="7231360"/>
+        <c:axId val="7232896"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="53106560"/>
+        <c:axId val="7231360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -992,7 +1004,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53108096"/>
+        <c:crossAx val="7232896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1000,7 +1012,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53108096"/>
+        <c:axId val="7232896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1016,7 +1028,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="53106560"/>
+        <c:crossAx val="7231360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1135,10 +1147,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>61.5</c:v>
+                  <c:v>67.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>48.5</c:v>
@@ -1157,12 +1169,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="53141504"/>
-        <c:axId val="53143040"/>
+        <c:axId val="7266304"/>
+        <c:axId val="7267840"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="53141504"/>
+        <c:axId val="7266304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1171,7 +1183,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53143040"/>
+        <c:crossAx val="7267840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1179,7 +1191,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53143040"/>
+        <c:axId val="7267840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1190,7 +1202,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53141504"/>
+        <c:crossAx val="7266304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1604,7 +1616,7 @@
       </c>
       <c r="B3" s="7">
         <f>SUM(B6,B12,B27)</f>
-        <v>90.5</v>
+        <v>98.5</v>
       </c>
       <c r="C3" s="27">
         <f>AVERAGE(C6,C12,C17,C22,C27)</f>
@@ -1742,7 +1754,7 @@
       </c>
       <c r="B12" s="17">
         <f>BacktestingSoftware!J6</f>
-        <v>87.5</v>
+        <v>95.5</v>
       </c>
       <c r="C12" s="29">
         <f>SUM(C13:C16)</f>
@@ -1809,7 +1821,7 @@
       </c>
       <c r="B16" s="19">
         <f>BacktestingSoftware!J5</f>
-        <v>12.5</v>
+        <v>20.5</v>
       </c>
       <c r="C16" s="31">
         <v>0</v>
@@ -2035,7 +2047,7 @@
       <c r="C34" s="48"/>
       <c r="D34" s="9">
         <f>SUM(Projektmanagment!I13,BacktestingSoftware!I13,Algorithmus!I13,Marktzustandserkennung!I13,Testing_Abschluss!I13)</f>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2045,7 +2057,7 @@
       <c r="C35" s="42"/>
       <c r="D35" s="9">
         <f>SUM(Projektmanagment!I14,BacktestingSoftware!I14,Algorithmus!I14,Marktzustandserkennung!I14,Testing_Abschluss!I14)</f>
-        <v>61.5</v>
+        <v>67.5</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2352,10 +2364,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2505,7 +2517,7 @@
       <c r="I5" s="61"/>
       <c r="J5" s="35">
         <f>SUMIF(B:B,H5,E:E)</f>
-        <v>12.5</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2533,7 +2545,7 @@
       <c r="I6" s="58"/>
       <c r="J6" s="7">
         <f>SUM(J2:J5)</f>
-        <v>87.5</v>
+        <v>95.5</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -2683,7 +2695,7 @@
       </c>
       <c r="I13" s="35">
         <f>SUMIF(A:A,H13,E:E)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -2710,7 +2722,7 @@
       </c>
       <c r="I14" s="35">
         <f>SUMIF(A:A,H14,E:E)</f>
-        <v>61.5</v>
+        <v>67.5</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2899,7 +2911,47 @@
         <v>4.5</v>
       </c>
       <c r="F23" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>125</v>
+      </c>
+      <c r="D24" s="1">
+        <v>41291</v>
+      </c>
+      <c r="E24" s="26">
+        <v>6</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D25" s="1">
+        <v>41291</v>
+      </c>
+      <c r="E25" s="26">
+        <v>2</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added dynamic indicator choosing, Added extended-WPF-Libraray, Corrected integration of trendstrengths
</commit_message>
<xml_diff>
--- a/Dokumentation/Noctua_Zeitaufzeichnung.xlsx
+++ b/Dokumentation/Noctua_Zeitaufzeichnung.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="48" yWindow="0" windowWidth="20736" windowHeight="11760" activeTab="2"/>
+    <workbookView xWindow="48" yWindow="0" windowWidth="20736" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Gesamtstatus" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="142">
   <si>
     <t>Arbeitspaket</t>
   </si>
@@ -432,6 +432,24 @@
   </si>
   <si>
     <t>Layout für Settings-Screen</t>
+  </si>
+  <si>
+    <t>Fertigstellung der Trendstärkenintegration</t>
+  </si>
+  <si>
+    <t>Trenstärkenintegration berichtigt</t>
+  </si>
+  <si>
+    <t>Trendstärken integriert 90%</t>
+  </si>
+  <si>
+    <t>Trendstärken integriert 100%</t>
+  </si>
+  <si>
+    <t>Möglichkeit zur Laufzeit dynamisch die gezeichneten Indikatoren zu bestimmten implementiert</t>
+  </si>
+  <si>
+    <t>#Indikatorenauswahl 80%</t>
   </si>
 </sst>
 </file>
@@ -1009,12 +1027,12 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:shape val="box"/>
-        <c:axId val="38007552"/>
-        <c:axId val="38009088"/>
+        <c:axId val="37779328"/>
+        <c:axId val="37780864"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="38007552"/>
+        <c:axId val="37779328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1023,7 +1041,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38009088"/>
+        <c:crossAx val="37780864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1031,7 +1049,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="38009088"/>
+        <c:axId val="37780864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1047,7 +1065,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="38007552"/>
+        <c:crossAx val="37779328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1170,7 +1188,7 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>67.5</c:v>
+                  <c:v>82.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>65</c:v>
@@ -1189,12 +1207,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="38087296"/>
-        <c:axId val="38113664"/>
+        <c:axId val="37801984"/>
+        <c:axId val="37803520"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="38087296"/>
+        <c:axId val="37801984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1203,7 +1221,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38113664"/>
+        <c:crossAx val="37803520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1211,7 +1229,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="38113664"/>
+        <c:axId val="37803520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1222,7 +1240,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38087296"/>
+        <c:crossAx val="37801984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1593,7 +1611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1636,7 +1654,7 @@
       </c>
       <c r="B3" s="7">
         <f>SUM(B6,B12,B27)</f>
-        <v>99.5</v>
+        <v>114.5</v>
       </c>
       <c r="C3" s="27">
         <f>AVERAGE(C6,C12,C17,C22,C27)</f>
@@ -1774,7 +1792,7 @@
       </c>
       <c r="B12" s="17">
         <f>BacktestingSoftware!J6</f>
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="C12" s="29">
         <f>SUM(C13:C16)</f>
@@ -1809,7 +1827,7 @@
       </c>
       <c r="B14" s="19">
         <f>BacktestingSoftware!J3</f>
-        <v>29.5</v>
+        <v>35.5</v>
       </c>
       <c r="C14" s="31">
         <v>0</v>
@@ -1841,7 +1859,7 @@
       </c>
       <c r="B16" s="19">
         <f>BacktestingSoftware!J5</f>
-        <v>20.5</v>
+        <v>29.5</v>
       </c>
       <c r="C16" s="31">
         <v>0</v>
@@ -2013,7 +2031,7 @@
       </c>
       <c r="D28" s="32"/>
     </row>
-    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="18" t="s">
         <v>23</v>
       </c>
@@ -2026,7 +2044,7 @@
       </c>
       <c r="D29" s="32"/>
     </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="18" t="s">
         <v>24</v>
       </c>
@@ -2039,7 +2057,7 @@
       </c>
       <c r="D30" s="32"/>
     </row>
-    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="20" t="s">
         <v>25</v>
       </c>
@@ -2052,15 +2070,15 @@
       </c>
       <c r="D31" s="28"/>
     </row>
-    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="33" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
       <c r="D33" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="47" t="s">
         <v>34</v>
       </c>
@@ -2070,17 +2088,17 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B35" s="41" t="s">
         <v>15</v>
       </c>
       <c r="C35" s="42"/>
       <c r="D35" s="9">
         <f>SUM(Projektmanagment!I14,BacktestingSoftware!I14,Algorithmus!I14,Marktzustandserkennung!I14,Testing_Abschluss!I14)</f>
-        <v>67.5</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>82.5</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B36" s="43" t="s">
         <v>35</v>
       </c>
@@ -2340,7 +2358,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D14" s="1"/>
       <c r="H14" s="33" t="s">
         <v>6</v>
@@ -2350,7 +2368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D15" s="1"/>
       <c r="H15" s="33" t="s">
         <v>33</v>
@@ -2360,15 +2378,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D16" s="1"/>
       <c r="H16" s="36"/>
       <c r="I16" s="36"/>
     </row>
-    <row r="17" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D18" s="1"/>
     </row>
   </sheetData>
@@ -2401,17 +2419,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="71.88671875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="66.21875" style="3" customWidth="1"/>
     <col min="4" max="4" width="10.88671875" style="3"/>
     <col min="5" max="5" width="10.88671875" style="26"/>
     <col min="6" max="6" width="24.44140625" style="3" customWidth="1"/>
@@ -2498,7 +2516,7 @@
       <c r="I3" s="61"/>
       <c r="J3" s="35">
         <f>SUMIF(B:B,H3,E:E)</f>
-        <v>29.5</v>
+        <v>35.5</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -2554,7 +2572,7 @@
       <c r="I5" s="61"/>
       <c r="J5" s="35">
         <f>SUMIF(B:B,H5,E:E)</f>
-        <v>20.5</v>
+        <v>29.5</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2582,7 +2600,7 @@
       <c r="I6" s="58"/>
       <c r="J6" s="7">
         <f>SUM(J2:J5)</f>
-        <v>96</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -2759,7 +2777,7 @@
       </c>
       <c r="I14" s="35">
         <f>SUMIF(A:A,H14,E:E)</f>
-        <v>67.5</v>
+        <v>82.5</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2811,7 +2829,7 @@
       <c r="H16" s="36"/>
       <c r="I16" s="36"/>
     </row>
-    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>6</v>
       </c>
@@ -2831,7 +2849,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>6</v>
       </c>
@@ -3012,7 +3030,64 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D27" s="1"/>
+      <c r="A27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D27" s="1">
+        <v>41297</v>
+      </c>
+      <c r="E27" s="26">
+        <v>4.5</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D28" s="1">
+        <v>41302</v>
+      </c>
+      <c r="E28" s="26">
+        <v>4.5</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D29" s="1">
+        <v>41303</v>
+      </c>
+      <c r="E29" s="26">
+        <v>6</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>141</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -3295,7 +3370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D14" s="1"/>
       <c r="H14" s="35" t="s">
         <v>6</v>
@@ -3305,7 +3380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D15" s="1"/>
       <c r="H15" s="35" t="s">
         <v>33</v>
@@ -3315,15 +3390,15 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D16" s="1"/>
       <c r="H16" s="36"/>
       <c r="I16" s="36"/>
     </row>
-    <row r="17" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D18" s="1"/>
     </row>
   </sheetData>
@@ -3572,7 +3647,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D14" s="1"/>
       <c r="H14" s="35" t="s">
         <v>6</v>
@@ -3582,7 +3657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D15" s="1"/>
       <c r="H15" s="35" t="s">
         <v>33</v>
@@ -3592,15 +3667,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D16" s="1"/>
       <c r="H16" s="36"/>
       <c r="I16" s="36"/>
     </row>
-    <row r="17" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D18" s="1"/>
     </row>
   </sheetData>
@@ -3743,10 +3818,10 @@
     <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D12" s="1"/>
       <c r="H12" s="34" t="s">
         <v>5</v>
@@ -3755,7 +3830,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D13" s="1"/>
       <c r="H13" s="35" t="s">
         <v>32</v>
@@ -3765,7 +3840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D14" s="1"/>
       <c r="H14" s="35" t="s">
         <v>6</v>
@@ -3775,7 +3850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D15" s="1"/>
       <c r="H15" s="35" t="s">
         <v>33</v>
@@ -3785,15 +3860,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D16" s="1"/>
       <c r="H16" s="36"/>
       <c r="I16" s="36"/>
     </row>
-    <row r="17" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D18" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Major Bugfixes in BacktestingSoftware
</commit_message>
<xml_diff>
--- a/Dokumentation/Noctua_Zeitaufzeichnung.xlsx
+++ b/Dokumentation/Noctua_Zeitaufzeichnung.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="10245" windowHeight="8310"/>
+    <workbookView xWindow="-12" yWindow="-12" windowWidth="10248" windowHeight="8316" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Gesamtstatus" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="173">
   <si>
     <t>Arbeitspaket</t>
   </si>
@@ -539,7 +539,10 @@
     <t>Bugfixes</t>
   </si>
   <si>
-    <t xml:space="preserve">Inputverarbeitung; Neutralpfeil (Farben) </t>
+    <t xml:space="preserve">Inputverarbeitung; Neutralpfeil (+Farben) </t>
+  </si>
+  <si>
+    <t>Multiple Starts &amp; Excpetionhandling</t>
   </si>
 </sst>
 </file>
@@ -1118,12 +1121,12 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:shape val="box"/>
-        <c:axId val="87858560"/>
-        <c:axId val="87864448"/>
+        <c:axId val="42104320"/>
+        <c:axId val="42105856"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="87858560"/>
+        <c:axId val="42104320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1132,7 +1135,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87864448"/>
+        <c:crossAx val="42105856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1140,7 +1143,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87864448"/>
+        <c:axId val="42105856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1156,7 +1159,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="87858560"/>
+        <c:crossAx val="42104320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1270,7 +1273,7 @@
                   <c:v>31.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>92.5</c:v>
+                  <c:v>95.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>104</c:v>
@@ -1289,12 +1292,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="93521024"/>
-        <c:axId val="93522560"/>
+        <c:axId val="42130432"/>
+        <c:axId val="42132224"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="93521024"/>
+        <c:axId val="42130432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1303,7 +1306,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93522560"/>
+        <c:crossAx val="42132224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1311,7 +1314,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93522560"/>
+        <c:axId val="42132224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1322,7 +1325,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93521024"/>
+        <c:crossAx val="42130432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1693,17 +1696,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="50"/>
       <c r="B1" s="52" t="s">
         <v>28</v>
@@ -1717,7 +1720,7 @@
       <c r="G1" s="12"/>
       <c r="R1" s="8"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="51"/>
       <c r="B2" s="53"/>
       <c r="C2" s="13" t="s">
@@ -1736,7 +1739,7 @@
       </c>
       <c r="B3" s="7">
         <f>SUM(B6,B12,B27)</f>
-        <v>125.5</v>
+        <v>128.5</v>
       </c>
       <c r="C3" s="27">
         <f>AVERAGE(C6,C12,C17,C22,C27)</f>
@@ -1749,7 +1752,7 @@
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="47"/>
       <c r="B4" s="52"/>
       <c r="C4" s="54" t="s">
@@ -1760,7 +1763,7 @@
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
     </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="51"/>
       <c r="B5" s="53"/>
       <c r="C5" s="56"/>
@@ -1769,7 +1772,7 @@
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>13</v>
       </c>
@@ -1788,7 +1791,7 @@
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>18</v>
       </c>
@@ -1804,7 +1807,7 @@
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>17</v>
       </c>
@@ -1820,7 +1823,7 @@
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>19</v>
       </c>
@@ -1836,7 +1839,7 @@
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>20</v>
       </c>
@@ -1868,13 +1871,13 @@
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>54</v>
       </c>
       <c r="B12" s="17">
         <f>BacktestingSoftware!J6</f>
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C12" s="29">
         <f>SUM(C13:C16)</f>
@@ -1887,7 +1890,7 @@
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>53</v>
       </c>
@@ -1903,7 +1906,7 @@
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>55</v>
       </c>
@@ -1919,7 +1922,7 @@
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>56</v>
       </c>
@@ -1941,14 +1944,14 @@
       </c>
       <c r="B16" s="19">
         <f>BacktestingSoftware!J5</f>
-        <v>39.5</v>
+        <v>42.5</v>
       </c>
       <c r="C16" s="31">
         <v>0</v>
       </c>
       <c r="D16" s="32"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>58</v>
       </c>
@@ -1964,7 +1967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>59</v>
       </c>
@@ -1977,7 +1980,7 @@
       </c>
       <c r="D18" s="32"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>60</v>
       </c>
@@ -1990,7 +1993,7 @@
       </c>
       <c r="D19" s="32"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>61</v>
       </c>
@@ -2016,7 +2019,7 @@
       </c>
       <c r="D21" s="32"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>63</v>
       </c>
@@ -2032,7 +2035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
         <v>59</v>
       </c>
@@ -2045,7 +2048,7 @@
       </c>
       <c r="D23" s="32"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
         <v>64</v>
       </c>
@@ -2084,7 +2087,7 @@
       </c>
       <c r="D26" s="32"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>14</v>
       </c>
@@ -2113,7 +2116,7 @@
       </c>
       <c r="D28" s="32"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
         <v>23</v>
       </c>
@@ -2126,7 +2129,7 @@
       </c>
       <c r="D29" s="32"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
         <v>24</v>
       </c>
@@ -2177,7 +2180,7 @@
       <c r="C35" s="43"/>
       <c r="D35" s="9">
         <f>SUM(Projektmanagment!I14,BacktestingSoftware!I14,Algorithmus!I14,Marktzustandserkennung!I14,Testing_Abschluss!I14)</f>
-        <v>92.5</v>
+        <v>95.5</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2220,15 +2223,15 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="71.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="3"/>
-    <col min="5" max="5" width="10.85546875" style="26"/>
-    <col min="6" max="6" width="24.42578125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="71.88671875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" style="3"/>
+    <col min="5" max="5" width="10.88671875" style="26"/>
+    <col min="6" max="6" width="24.44140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2258,7 +2261,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>32</v>
       </c>
@@ -2286,7 +2289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
@@ -2314,7 +2317,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>32</v>
       </c>
@@ -2342,7 +2345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>32</v>
       </c>
@@ -2426,7 +2429,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>32</v>
       </c>
@@ -2446,10 +2449,10 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2464,7 +2467,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D13" s="1"/>
       <c r="H13" s="33" t="s">
         <v>32</v>
@@ -2474,7 +2477,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D14" s="1"/>
       <c r="H14" s="33" t="s">
         <v>6</v>
@@ -2494,15 +2497,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D16" s="1"/>
       <c r="H16" s="36"/>
       <c r="I16" s="36"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
     </row>
   </sheetData>
@@ -2534,21 +2537,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="66.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="3"/>
-    <col min="5" max="5" width="10.85546875" style="26"/>
-    <col min="6" max="6" width="24.42578125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="66.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" style="3"/>
+    <col min="5" max="5" width="10.88671875" style="26"/>
+    <col min="6" max="6" width="24.44140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2578,7 +2581,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -2606,7 +2609,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>33</v>
       </c>
@@ -2634,7 +2637,7 @@
         <v>35.5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -2687,7 +2690,7 @@
       <c r="I5" s="62"/>
       <c r="J5" s="35">
         <f>SUMIF(B:B,H5,E:E)</f>
-        <v>39.5</v>
+        <v>42.5</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2715,10 +2718,10 @@
       <c r="I6" s="59"/>
       <c r="J6" s="7">
         <f>SUM(J2:J5)</f>
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>33</v>
       </c>
@@ -2738,7 +2741,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>33</v>
       </c>
@@ -2758,7 +2761,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
@@ -2778,7 +2781,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>32</v>
       </c>
@@ -2841,7 +2844,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>6</v>
       </c>
@@ -2868,7 +2871,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>33</v>
       </c>
@@ -2892,10 +2895,10 @@
       </c>
       <c r="I14" s="35">
         <f>SUMIF(A:A,H14,E:E)</f>
-        <v>92.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>95.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
@@ -2922,7 +2925,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>33</v>
       </c>
@@ -2944,7 +2947,7 @@
       <c r="H16" s="36"/>
       <c r="I16" s="36"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>6</v>
       </c>
@@ -2964,7 +2967,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>6</v>
       </c>
@@ -2984,7 +2987,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>6</v>
       </c>
@@ -3004,7 +3007,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>6</v>
       </c>
@@ -3024,7 +3027,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>6</v>
       </c>
@@ -3044,7 +3047,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>6</v>
       </c>
@@ -3064,7 +3067,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>6</v>
       </c>
@@ -3084,7 +3087,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>32</v>
       </c>
@@ -3104,7 +3107,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>6</v>
       </c>
@@ -3124,7 +3127,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>32</v>
       </c>
@@ -3144,7 +3147,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>6</v>
       </c>
@@ -3164,7 +3167,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>6</v>
       </c>
@@ -3184,7 +3187,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>6</v>
       </c>
@@ -3204,7 +3207,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>6</v>
       </c>
@@ -3224,7 +3227,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>6</v>
       </c>
@@ -3242,6 +3245,26 @@
       </c>
       <c r="F31" s="3" t="s">
         <v>171</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D32" s="1">
+        <v>41340</v>
+      </c>
+      <c r="E32" s="26">
+        <v>3</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -3278,15 +3301,15 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="71.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="3"/>
-    <col min="5" max="5" width="10.85546875" style="26"/>
-    <col min="6" max="6" width="24.42578125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="71.88671875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" style="3"/>
+    <col min="5" max="5" width="10.88671875" style="26"/>
+    <col min="6" max="6" width="24.44140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3316,7 +3339,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>33</v>
       </c>
@@ -3344,7 +3367,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>33</v>
       </c>
@@ -3372,7 +3395,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>33</v>
       </c>
@@ -3456,7 +3479,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>33</v>
       </c>
@@ -3476,7 +3499,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>33</v>
       </c>
@@ -3496,7 +3519,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>33</v>
       </c>
@@ -3516,7 +3539,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>33</v>
       </c>
@@ -3536,7 +3559,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>33</v>
       </c>
@@ -3556,7 +3579,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>33</v>
       </c>
@@ -3582,7 +3605,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
@@ -3609,7 +3632,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
@@ -3663,7 +3686,7 @@
         <v>64.5</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>32</v>
       </c>
@@ -3685,7 +3708,7 @@
       <c r="H16" s="36"/>
       <c r="I16" s="36"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>33</v>
       </c>
@@ -3705,7 +3728,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>32</v>
       </c>
@@ -3725,7 +3748,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>32</v>
       </c>
@@ -3745,7 +3768,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>33</v>
       </c>
@@ -3799,15 +3822,15 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="71.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" style="26"/>
-    <col min="6" max="6" width="24.42578125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.88671875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" style="26"/>
+    <col min="6" max="6" width="24.44140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3837,7 +3860,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>32</v>
       </c>
@@ -3865,7 +3888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>33</v>
       </c>
@@ -3893,7 +3916,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>33</v>
       </c>
@@ -3977,7 +4000,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>33</v>
       </c>
@@ -3997,7 +4020,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>33</v>
       </c>
@@ -4017,10 +4040,10 @@
         <v>167</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4035,7 +4058,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D13" s="1"/>
       <c r="H13" s="35" t="s">
         <v>32</v>
@@ -4045,7 +4068,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D14" s="1"/>
       <c r="H14" s="35" t="s">
         <v>6</v>
@@ -4065,15 +4088,15 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D16" s="1"/>
       <c r="H16" s="36"/>
       <c r="I16" s="36"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
     </row>
   </sheetData>
@@ -4110,15 +4133,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="71.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="3"/>
-    <col min="5" max="5" width="10.85546875" style="37"/>
-    <col min="6" max="6" width="24.42578125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="71.88671875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" style="3"/>
+    <col min="5" max="5" width="10.88671875" style="37"/>
+    <col min="6" max="6" width="24.44140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4148,7 +4171,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
       <c r="D2" s="1"/>
       <c r="H2" s="63" t="s">
@@ -4160,7 +4183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D3" s="1"/>
       <c r="H3" s="65" t="s">
         <v>50</v>
@@ -4171,7 +4194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D4" s="1"/>
       <c r="H4" s="65" t="s">
         <v>51</v>
@@ -4182,7 +4205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D5" s="1"/>
       <c r="H5" s="67" t="s">
         <v>52</v>
@@ -4204,16 +4227,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D8" s="24"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4228,7 +4251,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D13" s="1"/>
       <c r="H13" s="35" t="s">
         <v>32</v>
@@ -4238,7 +4261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D14" s="1"/>
       <c r="H14" s="35" t="s">
         <v>6</v>
@@ -4258,15 +4281,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D16" s="1"/>
       <c r="H16" s="36"/>
       <c r="I16" s="36"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
     </row>
   </sheetData>

</xml_diff>